<commit_message>
Did control signals for Arithmetics
</commit_message>
<xml_diff>
--- a/Project/ControlSignals.xlsx
+++ b/Project/ControlSignals.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction coding" sheetId="1" r:id="rId1"/>
-    <sheet name="Opcodes" sheetId="2" r:id="rId2"/>
+    <sheet name="Control Signals" sheetId="3" r:id="rId2"/>
+    <sheet name="Opcodes" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="124">
   <si>
     <t>OPCODE</t>
   </si>
@@ -238,9 +240,6 @@
     <t>01 0011</t>
   </si>
   <si>
-    <t>01 011</t>
-  </si>
-  <si>
     <t>01 0101</t>
   </si>
   <si>
@@ -320,13 +319,88 @@
   </si>
   <si>
     <t>brc ra &gt;= 0</t>
+  </si>
+  <si>
+    <t>STEP</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>OEN</t>
+  </si>
+  <si>
+    <t>WEN</t>
+  </si>
+  <si>
+    <t>FETCH</t>
+  </si>
+  <si>
+    <t>xx1x</t>
+  </si>
+  <si>
+    <t>STATE[4,1]</t>
+  </si>
+  <si>
+    <t>RegRd</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>xx00</t>
+  </si>
+  <si>
+    <t>RegWr</t>
+  </si>
+  <si>
+    <t>xxx0</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>xx01</t>
+  </si>
+  <si>
+    <t>x is don't care</t>
+  </si>
+  <si>
+    <t>inc rt, ra</t>
+  </si>
+  <si>
+    <t>subi rt, ra, imm</t>
+  </si>
+  <si>
+    <t>addi rt, ra, imm</t>
+  </si>
+  <si>
+    <t>sub rt, ra, rb</t>
+  </si>
+  <si>
+    <t>add rt, ra, rb</t>
+  </si>
+  <si>
+    <t>xx0x</t>
+  </si>
+  <si>
+    <t>1001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,8 +416,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,8 +468,14 @@
         <bgColor theme="4" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -591,11 +679,300 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -611,6 +988,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,18 +1003,86 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -974,6 +1425,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1700,10 +2152,1222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="9780"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="I24" sqref="I24"/>
+    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="55">
+        <v>0</v>
+      </c>
+      <c r="H3" s="56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0</v>
+      </c>
+      <c r="H4" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0</v>
+      </c>
+      <c r="H5" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="57"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="61">
+        <v>0</v>
+      </c>
+      <c r="H6" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G7" s="45">
+        <v>0</v>
+      </c>
+      <c r="H7" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="68"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="68"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0</v>
+      </c>
+      <c r="H9" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="70"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="61">
+        <v>0</v>
+      </c>
+      <c r="H10" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="45">
+        <v>0</v>
+      </c>
+      <c r="H11" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0</v>
+      </c>
+      <c r="H12" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0</v>
+      </c>
+      <c r="H13" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="57"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="61">
+        <v>0</v>
+      </c>
+      <c r="H14" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="45">
+        <v>0</v>
+      </c>
+      <c r="H15" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0</v>
+      </c>
+      <c r="H16" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="68"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="27">
+        <v>0</v>
+      </c>
+      <c r="H17" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="70"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="61">
+        <v>0</v>
+      </c>
+      <c r="H18" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="45">
+        <v>0</v>
+      </c>
+      <c r="H19" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="39"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="29">
+        <v>0</v>
+      </c>
+      <c r="H20" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" s="27">
+        <v>0</v>
+      </c>
+      <c r="H21" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="57"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="61">
+        <v>0</v>
+      </c>
+      <c r="H22" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="67"/>
+      <c r="D23" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" s="45">
+        <v>0</v>
+      </c>
+      <c r="H23" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="29">
+        <v>0</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="68"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="27">
+        <v>0</v>
+      </c>
+      <c r="H25" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="70"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="61">
+        <v>0</v>
+      </c>
+      <c r="H26" s="62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="43"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="46"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="32"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="33"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="30"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="31"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="32"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="33"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="30"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="31"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="32"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="33"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="30"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="31"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="32"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="33"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="30"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="31"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="32"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="33"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="30"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="31"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="32"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="33"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="30"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="31"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="32"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="33"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="30"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="31"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="32"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="33"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="30"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="31"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="32"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="33"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="30"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="31"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="32"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="33"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="30"/>
+      <c r="C47" s="41"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="31"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="32"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="33"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="30"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="31"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="32"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="33"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="30"/>
+      <c r="C51" s="41"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="31"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="32"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="33"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="30"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="31"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="32"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="33"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="30"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="31"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="32"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="33"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="30"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="31"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="32"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="33"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="30"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="31"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="32"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="28"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="33"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="30"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="31"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="32"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="33"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="30"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="31"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="32"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="33"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="30"/>
+      <c r="C65" s="41"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="31"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="32"/>
+      <c r="C66" s="42"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="33"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="30"/>
+      <c r="C67" s="41"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="26"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="31"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="32"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="33"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="30"/>
+      <c r="C69" s="41"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="31"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="32"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="33"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="34"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="31"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="35"/>
+      <c r="C72" s="42"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="33"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="34"/>
+      <c r="C73" s="41"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="27"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="31"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="35"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="35"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="33"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="34"/>
+      <c r="C75" s="41"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="31"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="35"/>
+      <c r="C76" s="42"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="33"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="34"/>
+      <c r="C77" s="41"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="31"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="35"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="33"/>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="34"/>
+      <c r="C79" s="41"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="27"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="31"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="35"/>
+      <c r="C80" s="42"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="33"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="34"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="31"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="35"/>
+      <c r="C82" s="42"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="33"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="34"/>
+      <c r="C83" s="41"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="31"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="35"/>
+      <c r="C84" s="42"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
+      <c r="H84" s="33"/>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="34"/>
+      <c r="C85" s="41"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="27"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="27"/>
+      <c r="H85" s="31"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="35"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="35"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="33"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="34"/>
+      <c r="C87" s="41"/>
+      <c r="D87" s="34"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="31"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="35"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="35"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="33"/>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="34"/>
+      <c r="C89" s="41"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="31"/>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="35"/>
+      <c r="C90" s="42"/>
+      <c r="D90" s="35"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="33"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="34"/>
+      <c r="C91" s="41"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="27"/>
+      <c r="H91" s="31"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="35"/>
+      <c r="C92" s="42"/>
+      <c r="D92" s="35"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="33"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="34"/>
+      <c r="C93" s="41"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="27"/>
+      <c r="H93" s="31"/>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="35"/>
+      <c r="C94" s="42"/>
+      <c r="D94" s="35"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="33"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="34"/>
+      <c r="C95" s="41"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
+      <c r="G95" s="27"/>
+      <c r="H95" s="31"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="35"/>
+      <c r="C96" s="42"/>
+      <c r="D96" s="35"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="33"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="34"/>
+      <c r="C97" s="41"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
+      <c r="G97" s="27"/>
+      <c r="H97" s="31"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="35"/>
+      <c r="C98" s="42"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
+      <c r="H98" s="33"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="34"/>
+      <c r="C99" s="41"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
+      <c r="G99" s="27"/>
+      <c r="H99" s="31"/>
+    </row>
+    <row r="100" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="36"/>
+      <c r="C100" s="63"/>
+      <c r="D100" s="36"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="38"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C15:C18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,7 +3380,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1744,7 +3408,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1758,7 +3422,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1770,7 +3434,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1782,7 +3446,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1794,7 +3458,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1806,19 +3470,19 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="17" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="22" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1832,7 +3496,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="5" t="s">
         <v>36</v>
       </c>
@@ -1844,7 +3508,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1856,7 +3520,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
@@ -1868,7 +3532,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1876,11 +3540,11 @@
         <v>29</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="5" t="s">
         <v>40</v>
       </c>
@@ -1888,11 +3552,11 @@
         <v>29</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
@@ -1900,11 +3564,11 @@
         <v>29</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="5" t="s">
         <v>42</v>
       </c>
@@ -1912,11 +3576,11 @@
         <v>43</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
@@ -1924,11 +3588,11 @@
         <v>43</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="5" t="s">
         <v>45</v>
       </c>
@@ -1936,23 +3600,23 @@
         <v>43</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+      <c r="C20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="23" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -1962,11 +3626,11 @@
         <v>32</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
@@ -1974,11 +3638,11 @@
         <v>50</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="5" t="s">
         <v>51</v>
       </c>
@@ -1986,11 +3650,11 @@
         <v>32</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="3" t="s">
         <v>52</v>
       </c>
@@ -1998,11 +3662,11 @@
         <v>53</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="5" t="s">
         <v>54</v>
       </c>
@@ -2010,11 +3674,11 @@
         <v>50</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="17"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="3" t="s">
         <v>55</v>
       </c>
@@ -2022,23 +3686,23 @@
         <v>32</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="17"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="22" t="s">
-        <v>84</v>
+      <c r="E27" s="17" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="22" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2048,91 +3712,91 @@
         <v>59</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="20"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="20"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="20"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="20"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>60</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="20"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="18"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>60</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Control Signals Table Done
</commit_message>
<xml_diff>
--- a/Project/ControlSignals.xlsx
+++ b/Project/ControlSignals.xlsx
@@ -4,7 +4,6 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="1"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="162">
   <si>
     <t>OPCODE</t>
   </si>
@@ -357,9 +356,6 @@
     <t>RegWr</t>
   </si>
   <si>
-    <t>xxx0</t>
-  </si>
-  <si>
     <t>1000</t>
   </si>
   <si>
@@ -394,6 +390,123 @@
   </si>
   <si>
     <t>1001</t>
+  </si>
+  <si>
+    <t>dec rt, ra</t>
+  </si>
+  <si>
+    <t>not  rt, ra</t>
+  </si>
+  <si>
+    <t>and rt, ra, rb</t>
+  </si>
+  <si>
+    <t>or rt, ra, rb</t>
+  </si>
+  <si>
+    <t>xor rt, ra, rb</t>
+  </si>
+  <si>
+    <t>andi rt, ra, imm</t>
+  </si>
+  <si>
+    <t>ori rt, ra, imm</t>
+  </si>
+  <si>
+    <t>xori rt, ra, imm</t>
+  </si>
+  <si>
+    <t>shl rt, ra, n</t>
+  </si>
+  <si>
+    <t>shr rt, ra, n</t>
+  </si>
+  <si>
+    <t>rotl rt, ra, n</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>0110</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>01 0100</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>move rt, ra</t>
+  </si>
+  <si>
+    <t>0xxx</t>
+  </si>
+  <si>
+    <t>loadi rt, imm</t>
+  </si>
+  <si>
+    <t>MemAcc</t>
+  </si>
+  <si>
+    <t>x1xx</t>
+  </si>
+  <si>
+    <t>1xxx</t>
+  </si>
+  <si>
+    <t>loadr rt, ra</t>
+  </si>
+  <si>
+    <t>x0xx</t>
+  </si>
+  <si>
+    <t>Regwr</t>
+  </si>
+  <si>
+    <t>loado rt, ra, off</t>
+  </si>
+  <si>
+    <t>rb,imm</t>
+  </si>
+  <si>
+    <t>rb,ra</t>
+  </si>
+  <si>
+    <t>rb,ra,off</t>
+  </si>
+  <si>
+    <t>stori rb, imm</t>
+  </si>
+  <si>
+    <t>storr rb, ra</t>
+  </si>
+  <si>
+    <t>storo rb, ra, off</t>
+  </si>
+  <si>
+    <t>xx11</t>
+  </si>
+  <si>
+    <t>11 0ccc</t>
   </si>
 </sst>
 </file>
@@ -475,7 +588,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -968,11 +1081,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -994,6 +1170,72 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1009,80 +1251,108 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,10 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC15" sqref="AC15"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2152,14 +2419,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H100"/>
+  <dimension ref="B1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9780"/>
-      <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="I24" sqref="I24"/>
-    </sheetView>
-    <sheetView zoomScaleNormal="100" workbookViewId="1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2171,1176 +2433,2300 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="39">
+        <v>0</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="46"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0</v>
+      </c>
+      <c r="H4" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="46"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="22">
+        <v>0</v>
+      </c>
+      <c r="H5" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="47"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="43">
+        <v>0</v>
+      </c>
+      <c r="H6" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="32">
+        <v>0</v>
+      </c>
+      <c r="H7" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="49"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="49"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="22">
+        <v>0</v>
+      </c>
+      <c r="H9" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="50"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="43">
+        <v>0</v>
+      </c>
+      <c r="H10" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" s="32">
+        <v>0</v>
+      </c>
+      <c r="H11" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="46"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="46"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="22">
+        <v>0</v>
+      </c>
+      <c r="H13" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="43">
+        <v>0</v>
+      </c>
+      <c r="H14" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" s="32">
+        <v>0</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="49"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0</v>
+      </c>
+      <c r="H16" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="49"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="22">
+        <v>0</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="50"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="43">
+        <v>0</v>
+      </c>
+      <c r="H18" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="45" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="48" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="C19" s="51"/>
+      <c r="D19" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G19" s="32">
+        <v>0</v>
+      </c>
+      <c r="H19" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="46"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" s="24">
+        <v>0</v>
+      </c>
+      <c r="H20" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="53" t="s">
+      <c r="F21" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="22">
+        <v>0</v>
+      </c>
+      <c r="H21" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="43">
+        <v>0</v>
+      </c>
+      <c r="H22" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="54"/>
+      <c r="D23" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E23" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F23" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="32">
+        <v>0</v>
+      </c>
+      <c r="H23" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="49"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="49"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" s="22">
+        <v>0</v>
+      </c>
+      <c r="H25" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="50"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="43">
+        <v>0</v>
+      </c>
+      <c r="H26" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="32">
+        <v>0</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="46"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" s="24">
+        <v>0</v>
+      </c>
+      <c r="H28" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="46"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G29" s="22">
+        <v>0</v>
+      </c>
+      <c r="H29" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="47"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" s="43">
+        <v>0</v>
+      </c>
+      <c r="H30" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" s="32">
+        <v>0</v>
+      </c>
+      <c r="H31" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="49"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="24">
+        <v>0</v>
+      </c>
+      <c r="H32" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="49"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" s="22">
+        <v>0</v>
+      </c>
+      <c r="H33" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="50"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="43">
+        <v>0</v>
+      </c>
+      <c r="H34" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="32">
+        <v>0</v>
+      </c>
+      <c r="H35" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="46"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="24">
+        <v>0</v>
+      </c>
+      <c r="H36" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="46"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G37" s="22">
+        <v>0</v>
+      </c>
+      <c r="H37" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="47"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="43">
+        <v>0</v>
+      </c>
+      <c r="H38" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G39" s="32">
+        <v>0</v>
+      </c>
+      <c r="H39" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="49"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="24">
+        <v>0</v>
+      </c>
+      <c r="H40" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="49"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="G41" s="22">
+        <v>0</v>
+      </c>
+      <c r="H41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="50"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42" s="43">
+        <v>0</v>
+      </c>
+      <c r="H42" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="51" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G43" s="32">
+        <v>0</v>
+      </c>
+      <c r="H43" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="46"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="24">
+        <v>0</v>
+      </c>
+      <c r="H44" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="46"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="G45" s="22">
+        <v>0</v>
+      </c>
+      <c r="H45" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="47"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F46" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G46" s="43">
+        <v>0</v>
+      </c>
+      <c r="H46" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" s="32">
+        <v>0</v>
+      </c>
+      <c r="H47" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="49"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" s="24">
+        <v>0</v>
+      </c>
+      <c r="H48" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="49"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G49" s="22">
+        <v>0</v>
+      </c>
+      <c r="H49" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="50"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G50" s="43">
+        <v>0</v>
+      </c>
+      <c r="H50" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G51" s="32">
+        <v>0</v>
+      </c>
+      <c r="H51" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="46"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G52" s="24">
+        <v>0</v>
+      </c>
+      <c r="H52" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="46"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="G53" s="22">
+        <v>0</v>
+      </c>
+      <c r="H53" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="47"/>
+      <c r="C54" s="53"/>
+      <c r="D54" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E54" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F54" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G54" s="43">
+        <v>0</v>
+      </c>
+      <c r="H54" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C55" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G55" s="32">
+        <v>0</v>
+      </c>
+      <c r="H55" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="49"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G56" s="24">
+        <v>0</v>
+      </c>
+      <c r="H56" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="49"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="G57" s="22">
+        <v>0</v>
+      </c>
+      <c r="H57" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="50"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E58" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F58" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G58" s="43">
+        <v>0</v>
+      </c>
+      <c r="H58" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E59" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G59" s="32">
+        <v>0</v>
+      </c>
+      <c r="H59" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="46"/>
+      <c r="C60" s="52"/>
+      <c r="D60" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G60" s="24">
+        <v>0</v>
+      </c>
+      <c r="H60" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="46"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="G61" s="22">
+        <v>0</v>
+      </c>
+      <c r="H61" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="47"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E62" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G62" s="43">
+        <v>0</v>
+      </c>
+      <c r="H62" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F63" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G63" s="32">
+        <v>0</v>
+      </c>
+      <c r="H63" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="49"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G64" s="24">
+        <v>0</v>
+      </c>
+      <c r="H64" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="49"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="G65" s="22">
+        <v>0</v>
+      </c>
+      <c r="H65" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="50"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F66" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G66" s="43">
+        <v>0</v>
+      </c>
+      <c r="H66" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F67" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G67" s="32">
+        <v>0</v>
+      </c>
+      <c r="H67" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="46"/>
+      <c r="C68" s="52"/>
+      <c r="D68" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E68" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F68" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G68" s="24">
+        <v>0</v>
+      </c>
+      <c r="H68" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="46"/>
+      <c r="C69" s="52"/>
+      <c r="D69" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="G69" s="22">
+        <v>0</v>
+      </c>
+      <c r="H69" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="47"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E70" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F70" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="G70" s="43">
+        <v>0</v>
+      </c>
+      <c r="H70" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="103" t="s">
+        <v>144</v>
+      </c>
+      <c r="C71" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="D71" s="77" t="s">
+        <v>103</v>
+      </c>
+      <c r="E71" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="F71" s="79">
+        <v>1000</v>
+      </c>
+      <c r="G71" s="78">
+        <v>0</v>
+      </c>
+      <c r="H71" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="104"/>
+      <c r="C72" s="55"/>
+      <c r="D72" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="E72" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G72" s="24">
+        <v>0</v>
+      </c>
+      <c r="H72" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="104"/>
+      <c r="C73" s="55"/>
+      <c r="D73" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E73" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="G73" s="69">
+        <v>0</v>
+      </c>
+      <c r="H73" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="105"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E74" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F74" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G74" s="82">
+        <v>0</v>
+      </c>
+      <c r="H74" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="106" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" s="107" t="s">
+        <v>79</v>
+      </c>
+      <c r="D75" s="90" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="F75" s="79">
+        <v>1000</v>
+      </c>
+      <c r="G75" s="78">
+        <v>0</v>
+      </c>
+      <c r="H75" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="108"/>
+      <c r="C76" s="109"/>
+      <c r="D76" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="E76" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F76" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G76" s="71">
+        <v>0</v>
+      </c>
+      <c r="H76" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="110"/>
+      <c r="C77" s="111"/>
+      <c r="D77" s="93" t="s">
+        <v>110</v>
+      </c>
+      <c r="E77" s="94" t="s">
+        <v>149</v>
+      </c>
+      <c r="F77" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="G77" s="95">
+        <v>0</v>
+      </c>
+      <c r="H77" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="103" t="s">
+        <v>150</v>
+      </c>
+      <c r="C78" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="D78" s="97" t="s">
+        <v>103</v>
+      </c>
+      <c r="E78" s="98" t="s">
+        <v>104</v>
+      </c>
+      <c r="F78" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="G78" s="99">
+        <v>0</v>
+      </c>
+      <c r="H78" s="100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="104"/>
+      <c r="C79" s="55"/>
+      <c r="D79" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E79" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F79" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G79" s="73">
+        <v>0</v>
+      </c>
+      <c r="H79" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="104"/>
+      <c r="C80" s="55"/>
+      <c r="D80" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E80" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="F80" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G80" s="71">
+        <v>0</v>
+      </c>
+      <c r="H80" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="104"/>
+      <c r="C81" s="55"/>
+      <c r="D81" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G81" s="73">
+        <v>0</v>
+      </c>
+      <c r="H81" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="105"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E82" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="F82" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G82" s="82">
+        <v>0</v>
+      </c>
+      <c r="H82" s="83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="C83" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G83" s="75">
+        <v>0</v>
+      </c>
+      <c r="H83" s="76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="66"/>
+      <c r="C84" s="52"/>
+      <c r="D84" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E84" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F84" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G84" s="71">
+        <v>0</v>
+      </c>
+      <c r="H84" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" s="66"/>
+      <c r="C85" s="52"/>
+      <c r="D85" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F85" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="55">
-        <v>0</v>
-      </c>
-      <c r="H3" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="32" t="s">
+      <c r="G85" s="73">
+        <v>0</v>
+      </c>
+      <c r="H85" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="66"/>
+      <c r="C86" s="52"/>
+      <c r="D86" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="E86" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F86" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G86" s="71">
+        <v>0</v>
+      </c>
+      <c r="H86" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="81"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E87" s="94" t="s">
+        <v>149</v>
+      </c>
+      <c r="F87" s="94" t="s">
+        <v>107</v>
+      </c>
+      <c r="G87" s="95">
+        <v>0</v>
+      </c>
+      <c r="H87" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="84" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="D88" s="86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E88" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="F88" s="87" t="s">
+        <v>111</v>
+      </c>
+      <c r="G88" s="88">
+        <v>0</v>
+      </c>
+      <c r="H88" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="67"/>
+      <c r="C89" s="68"/>
+      <c r="D89" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="29">
-        <v>0</v>
-      </c>
-      <c r="H4" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="30" t="s">
+      <c r="E89" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G89" s="73">
+        <v>0</v>
+      </c>
+      <c r="H89" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B90" s="91"/>
+      <c r="C90" s="92"/>
+      <c r="D90" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E90" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F90" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G90" s="82">
+        <v>1</v>
+      </c>
+      <c r="H90" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="C91" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E91" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F91" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G91" s="75">
+        <v>0</v>
+      </c>
+      <c r="H91" s="76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="66"/>
+      <c r="C92" s="52"/>
+      <c r="D92" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E92" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F92" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G92" s="71">
+        <v>0</v>
+      </c>
+      <c r="H92" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="66"/>
+      <c r="C93" s="52"/>
+      <c r="D93" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E5" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="27">
-        <v>0</v>
-      </c>
-      <c r="H5" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="57"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" s="60" t="s">
+      <c r="E93" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="G93" s="73">
+        <v>0</v>
+      </c>
+      <c r="H93" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="81"/>
+      <c r="C94" s="53"/>
+      <c r="D94" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E94" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F94" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G94" s="82">
+        <v>1</v>
+      </c>
+      <c r="H94" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B95" s="103" t="s">
+        <v>159</v>
+      </c>
+      <c r="C95" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="D95" s="90" t="s">
+        <v>103</v>
+      </c>
+      <c r="E95" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="F95" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6" s="61">
-        <v>0</v>
-      </c>
-      <c r="H6" s="62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="66" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="43" t="s">
+      <c r="G95" s="101">
+        <v>0</v>
+      </c>
+      <c r="H95" s="102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B96" s="104"/>
+      <c r="C96" s="55"/>
+      <c r="D96" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E96" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F96" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G96" s="71">
+        <v>0</v>
+      </c>
+      <c r="H96" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="104"/>
+      <c r="C97" s="55"/>
+      <c r="D97" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E97" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F97" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G97" s="73">
+        <v>0</v>
+      </c>
+      <c r="H97" s="74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="105"/>
+      <c r="C98" s="56"/>
+      <c r="D98" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E98" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="F98" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="G98" s="82">
+        <v>1</v>
+      </c>
+      <c r="H98" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="D99" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E99" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F99" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="G99" s="101">
+        <v>0</v>
+      </c>
+      <c r="H99" s="102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="81"/>
+      <c r="C100" s="53"/>
+      <c r="D100" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E100" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F100" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="G7" s="45">
-        <v>0</v>
-      </c>
-      <c r="H7" s="46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="32" t="s">
+      <c r="G100" s="82">
+        <v>0</v>
+      </c>
+      <c r="H100" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101" s="85" t="s">
+        <v>161</v>
+      </c>
+      <c r="D101" s="112" t="s">
+        <v>103</v>
+      </c>
+      <c r="E101" s="79" t="s">
+        <v>104</v>
+      </c>
+      <c r="F101" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="G101" s="101">
+        <v>0</v>
+      </c>
+      <c r="H101" s="102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="67"/>
+      <c r="C102" s="68"/>
+      <c r="D102" s="113" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="29">
-        <v>0</v>
-      </c>
-      <c r="H8" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="68"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="30" t="s">
+      <c r="E102" s="114" t="s">
+        <v>107</v>
+      </c>
+      <c r="F102" s="114" t="s">
+        <v>107</v>
+      </c>
+      <c r="G102" s="115">
+        <v>0</v>
+      </c>
+      <c r="H102" s="116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="120"/>
+      <c r="C103" s="121"/>
+      <c r="D103" s="122" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="27">
-        <v>0</v>
-      </c>
-      <c r="H9" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="70"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10" s="61">
-        <v>0</v>
-      </c>
-      <c r="H10" s="62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="G11" s="45">
-        <v>0</v>
-      </c>
-      <c r="H11" s="46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12" s="29">
-        <v>0</v>
-      </c>
-      <c r="H12" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" s="27">
-        <v>0</v>
-      </c>
-      <c r="H13" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="F14" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="61">
-        <v>0</v>
-      </c>
-      <c r="H14" s="62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="66" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="45">
-        <v>0</v>
-      </c>
-      <c r="H15" s="46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="68"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16" s="29">
-        <v>0</v>
-      </c>
-      <c r="H16" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" s="27">
-        <v>0</v>
-      </c>
-      <c r="H17" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="70"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18" s="61">
-        <v>0</v>
-      </c>
-      <c r="H18" s="62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" s="45">
-        <v>0</v>
-      </c>
-      <c r="H19" s="46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="29">
-        <v>0</v>
-      </c>
-      <c r="H20" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="G21" s="27">
-        <v>0</v>
-      </c>
-      <c r="H21" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="57"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="F22" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="61">
-        <v>0</v>
-      </c>
-      <c r="H22" s="62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="G23" s="45">
-        <v>0</v>
-      </c>
-      <c r="H23" s="46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="68"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="29">
-        <v>0</v>
-      </c>
-      <c r="H24" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="G25" s="27">
-        <v>0</v>
-      </c>
-      <c r="H25" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="70"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="E26" s="60" t="s">
-        <v>111</v>
-      </c>
-      <c r="F26" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="61">
-        <v>0</v>
-      </c>
-      <c r="H26" s="62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="43"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="46"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="32"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="33"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="30"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="31"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="32"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="33"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="30"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="31"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="32"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="33"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="30"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="31"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="32"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="33"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="30"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="31"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="32"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="33"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="30"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="31"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="32"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="33"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="30"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="31"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="32"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="33"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="30"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="31"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="32"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="33"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="31"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="32"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="33"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="31"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="32"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="33"/>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="30"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="31"/>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="32"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="33"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="30"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="31"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="32"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="33"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="30"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="30"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="31"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="32"/>
-      <c r="C52" s="42"/>
-      <c r="D52" s="32"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="33"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="30"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="31"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="32"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="33"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="30"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="31"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="32"/>
-      <c r="C56" s="42"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="33"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="30"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="31"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="32"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="33"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="30"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="31"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="32"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="33"/>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="30"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="31"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="32"/>
-      <c r="C62" s="42"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="33"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="30"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="26"/>
-      <c r="G63" s="27"/>
-      <c r="H63" s="31"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="32"/>
-      <c r="C64" s="42"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="33"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="30"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="30"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="26"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="31"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="32"/>
-      <c r="C66" s="42"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="33"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="30"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="26"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="31"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="32"/>
-      <c r="C68" s="42"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="33"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="30"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="30"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="26"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="31"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="32"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="33"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="34"/>
-      <c r="C71" s="41"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
-      <c r="H71" s="31"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="35"/>
-      <c r="C72" s="42"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="33"/>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="34"/>
-      <c r="C73" s="41"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="27"/>
-      <c r="H73" s="31"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="35"/>
-      <c r="C74" s="42"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="29"/>
-      <c r="F74" s="29"/>
-      <c r="G74" s="29"/>
-      <c r="H74" s="33"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="34"/>
-      <c r="C75" s="41"/>
-      <c r="D75" s="34"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="31"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="35"/>
-      <c r="C76" s="42"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="29"/>
-      <c r="F76" s="29"/>
-      <c r="G76" s="29"/>
-      <c r="H76" s="33"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="34"/>
-      <c r="C77" s="41"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="27"/>
-      <c r="H77" s="31"/>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="35"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="33"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="34"/>
-      <c r="C79" s="41"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="27"/>
-      <c r="H79" s="31"/>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="35"/>
-      <c r="C80" s="42"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="29"/>
-      <c r="G80" s="29"/>
-      <c r="H80" s="33"/>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="34"/>
-      <c r="C81" s="41"/>
-      <c r="D81" s="34"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="31"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="35"/>
-      <c r="C82" s="42"/>
-      <c r="D82" s="35"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
-      <c r="G82" s="29"/>
-      <c r="H82" s="33"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="34"/>
-      <c r="C83" s="41"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="31"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="35"/>
-      <c r="C84" s="42"/>
-      <c r="D84" s="35"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
-      <c r="G84" s="29"/>
-      <c r="H84" s="33"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="34"/>
-      <c r="C85" s="41"/>
-      <c r="D85" s="34"/>
-      <c r="E85" s="27"/>
-      <c r="F85" s="27"/>
-      <c r="G85" s="27"/>
-      <c r="H85" s="31"/>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="35"/>
-      <c r="C86" s="42"/>
-      <c r="D86" s="35"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
-      <c r="G86" s="29"/>
-      <c r="H86" s="33"/>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="34"/>
-      <c r="C87" s="41"/>
-      <c r="D87" s="34"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="27"/>
-      <c r="H87" s="31"/>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="35"/>
-      <c r="C88" s="42"/>
-      <c r="D88" s="35"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="29"/>
-      <c r="G88" s="29"/>
-      <c r="H88" s="33"/>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="34"/>
-      <c r="C89" s="41"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="31"/>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="35"/>
-      <c r="C90" s="42"/>
-      <c r="D90" s="35"/>
-      <c r="E90" s="29"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="29"/>
-      <c r="H90" s="33"/>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="34"/>
-      <c r="C91" s="41"/>
-      <c r="D91" s="34"/>
-      <c r="E91" s="27"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="27"/>
-      <c r="H91" s="31"/>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="35"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="35"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
-      <c r="G92" s="29"/>
-      <c r="H92" s="33"/>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="34"/>
-      <c r="C93" s="41"/>
-      <c r="D93" s="34"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="31"/>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="35"/>
-      <c r="C94" s="42"/>
-      <c r="D94" s="35"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="29"/>
-      <c r="G94" s="29"/>
-      <c r="H94" s="33"/>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="34"/>
-      <c r="C95" s="41"/>
-      <c r="D95" s="34"/>
-      <c r="E95" s="27"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="27"/>
-      <c r="H95" s="31"/>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="35"/>
-      <c r="C96" s="42"/>
-      <c r="D96" s="35"/>
-      <c r="E96" s="29"/>
-      <c r="F96" s="29"/>
-      <c r="G96" s="29"/>
-      <c r="H96" s="33"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="34"/>
-      <c r="C97" s="41"/>
-      <c r="D97" s="34"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="31"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="35"/>
-      <c r="C98" s="42"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="29"/>
-      <c r="F98" s="29"/>
-      <c r="G98" s="29"/>
-      <c r="H98" s="33"/>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="34"/>
-      <c r="C99" s="41"/>
-      <c r="D99" s="34"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="31"/>
-    </row>
-    <row r="100" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="36"/>
-      <c r="C100" s="63"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
-      <c r="G100" s="37"/>
-      <c r="H100" s="38"/>
+      <c r="E103" s="123" t="s">
+        <v>121</v>
+      </c>
+      <c r="F103" s="123" t="s">
+        <v>143</v>
+      </c>
+      <c r="G103" s="124">
+        <v>0</v>
+      </c>
+      <c r="H103" s="125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="117"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="118"/>
+      <c r="E104" s="118"/>
+      <c r="F104" s="118"/>
+      <c r="G104" s="119"/>
+      <c r="H104" s="119"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="117"/>
+      <c r="C105" s="118"/>
+      <c r="D105" s="118"/>
+      <c r="E105" s="118"/>
+      <c r="F105" s="118"/>
+      <c r="G105" s="119"/>
+      <c r="H105" s="119"/>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="117"/>
+      <c r="C106" s="118"/>
+      <c r="D106" s="118"/>
+      <c r="E106" s="118"/>
+      <c r="F106" s="118"/>
+      <c r="G106" s="119"/>
+      <c r="H106" s="119"/>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="117"/>
+      <c r="C107" s="118"/>
+      <c r="D107" s="118"/>
+      <c r="E107" s="118"/>
+      <c r="F107" s="118"/>
+      <c r="G107" s="119"/>
+      <c r="H107" s="119"/>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="117"/>
+      <c r="C108" s="118"/>
+      <c r="D108" s="118"/>
+      <c r="E108" s="118"/>
+      <c r="F108" s="118"/>
+      <c r="G108" s="119"/>
+      <c r="H108" s="119"/>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="117"/>
+      <c r="C109" s="118"/>
+      <c r="D109" s="118"/>
+      <c r="E109" s="118"/>
+      <c r="F109" s="118"/>
+      <c r="G109" s="119"/>
+      <c r="H109" s="119"/>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="117"/>
+      <c r="C110" s="118"/>
+      <c r="D110" s="118"/>
+      <c r="E110" s="118"/>
+      <c r="F110" s="118"/>
+      <c r="G110" s="119"/>
+      <c r="H110" s="119"/>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="117"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="118"/>
+      <c r="E111" s="118"/>
+      <c r="F111" s="118"/>
+      <c r="G111" s="119"/>
+      <c r="H111" s="119"/>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="117"/>
+      <c r="C112" s="118"/>
+      <c r="D112" s="118"/>
+      <c r="E112" s="118"/>
+      <c r="F112" s="118"/>
+      <c r="G112" s="119"/>
+      <c r="H112" s="119"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="117"/>
+      <c r="C113" s="118"/>
+      <c r="D113" s="118"/>
+      <c r="E113" s="118"/>
+      <c r="F113" s="118"/>
+      <c r="G113" s="119"/>
+      <c r="H113" s="119"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114" s="117"/>
+      <c r="C114" s="118"/>
+      <c r="D114" s="118"/>
+      <c r="E114" s="118"/>
+      <c r="F114" s="118"/>
+      <c r="G114" s="119"/>
+      <c r="H114" s="119"/>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" s="117"/>
+      <c r="C115" s="118"/>
+      <c r="D115" s="118"/>
+      <c r="E115" s="118"/>
+      <c r="F115" s="118"/>
+      <c r="G115" s="119"/>
+      <c r="H115" s="119"/>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="117"/>
+      <c r="C116" s="118"/>
+      <c r="D116" s="118"/>
+      <c r="E116" s="118"/>
+      <c r="F116" s="118"/>
+      <c r="G116" s="119"/>
+      <c r="H116" s="119"/>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117" s="117"/>
+      <c r="C117" s="118"/>
+      <c r="D117" s="118"/>
+      <c r="E117" s="118"/>
+      <c r="F117" s="118"/>
+      <c r="G117" s="119"/>
+      <c r="H117" s="119"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="117"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="118"/>
+      <c r="E118" s="118"/>
+      <c r="F118" s="118"/>
+      <c r="G118" s="119"/>
+      <c r="H118" s="119"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B119" s="117"/>
+      <c r="C119" s="118"/>
+      <c r="D119" s="118"/>
+      <c r="E119" s="118"/>
+      <c r="F119" s="118"/>
+      <c r="G119" s="119"/>
+      <c r="H119" s="119"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B120" s="117"/>
+      <c r="C120" s="118"/>
+      <c r="D120" s="118"/>
+      <c r="E120" s="118"/>
+      <c r="F120" s="118"/>
+      <c r="G120" s="119"/>
+      <c r="H120" s="119"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="117"/>
+      <c r="C121" s="118"/>
+      <c r="D121" s="118"/>
+      <c r="E121" s="118"/>
+      <c r="F121" s="118"/>
+      <c r="G121" s="119"/>
+      <c r="H121" s="119"/>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="117"/>
+      <c r="C122" s="118"/>
+      <c r="D122" s="118"/>
+      <c r="E122" s="118"/>
+      <c r="F122" s="118"/>
+      <c r="G122" s="119"/>
+      <c r="H122" s="119"/>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="117"/>
+      <c r="C123" s="118"/>
+      <c r="D123" s="118"/>
+      <c r="E123" s="118"/>
+      <c r="F123" s="118"/>
+      <c r="G123" s="119"/>
+      <c r="H123" s="119"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="117"/>
+      <c r="C124" s="118"/>
+      <c r="D124" s="118"/>
+      <c r="E124" s="118"/>
+      <c r="F124" s="118"/>
+      <c r="G124" s="119"/>
+      <c r="H124" s="119"/>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="117"/>
+      <c r="C125" s="118"/>
+      <c r="D125" s="118"/>
+      <c r="E125" s="118"/>
+      <c r="F125" s="118"/>
+      <c r="G125" s="119"/>
+      <c r="H125" s="119"/>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="117"/>
+      <c r="C126" s="118"/>
+      <c r="D126" s="118"/>
+      <c r="E126" s="118"/>
+      <c r="F126" s="118"/>
+      <c r="G126" s="119"/>
+      <c r="H126" s="119"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="52">
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B46"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C19:C22"/>
@@ -3356,6 +4742,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F73" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -3363,11 +4752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,7 +4794,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="59" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -3422,7 +4808,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="21"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
@@ -3434,7 +4820,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
@@ -3446,7 +4832,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
@@ -3458,7 +4844,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
@@ -3470,7 +4856,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="10" t="s">
         <v>33</v>
       </c>
@@ -3482,7 +4868,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="60" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -3496,7 +4882,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="5" t="s">
         <v>36</v>
       </c>
@@ -3508,7 +4894,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
@@ -3520,7 +4906,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
@@ -3532,7 +4918,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="3" t="s">
         <v>39</v>
       </c>
@@ -3540,11 +4926,11 @@
         <v>29</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="5" t="s">
         <v>40</v>
       </c>
@@ -3556,7 +4942,7 @@
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
@@ -3568,7 +4954,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="5" t="s">
         <v>42</v>
       </c>
@@ -3580,7 +4966,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
@@ -3592,7 +4978,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="5" t="s">
         <v>45</v>
       </c>
@@ -3604,7 +4990,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
+      <c r="B20" s="60"/>
       <c r="C20" s="18" t="s">
         <v>46</v>
       </c>
@@ -3616,7 +5002,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="61" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -3630,7 +5016,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="3" t="s">
         <v>49</v>
       </c>
@@ -3642,7 +5028,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="5" t="s">
         <v>51</v>
       </c>
@@ -3654,7 +5040,7 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="3" t="s">
         <v>52</v>
       </c>
@@ -3666,43 +5052,43 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="23"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>53</v>
+        <v>156</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="60" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -3716,7 +5102,7 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="24"/>
+      <c r="B29" s="62"/>
       <c r="C29" s="5" t="s">
         <v>92</v>
       </c>
@@ -3728,7 +5114,7 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="24"/>
+      <c r="B30" s="62"/>
       <c r="C30" s="3" t="s">
         <v>93</v>
       </c>
@@ -3740,7 +5126,7 @@
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="24"/>
+      <c r="B31" s="62"/>
       <c r="C31" s="5" t="s">
         <v>94</v>
       </c>
@@ -3752,7 +5138,7 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="24"/>
+      <c r="B32" s="62"/>
       <c r="C32" s="3" t="s">
         <v>95</v>
       </c>
@@ -3764,7 +5150,7 @@
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="24"/>
+      <c r="B33" s="62"/>
       <c r="C33" s="5" t="s">
         <v>96</v>
       </c>
@@ -3776,7 +5162,7 @@
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="24"/>
+      <c r="B34" s="62"/>
       <c r="C34" s="3" t="s">
         <v>97</v>
       </c>
@@ -3788,7 +5174,7 @@
       </c>
     </row>
     <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="25"/>
+      <c r="B35" s="63"/>
       <c r="C35" s="7" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
Back to work on this, after control
</commit_message>
<xml_diff>
--- a/Project/ControlSignals.xlsx
+++ b/Project/ControlSignals.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="168">
   <si>
     <t>OPCODE</t>
   </si>
@@ -507,6 +507,24 @@
   </si>
   <si>
     <t>11 0ccc</t>
+  </si>
+  <si>
+    <t>000100</t>
+  </si>
+  <si>
+    <t>000101</t>
+  </si>
+  <si>
+    <t>000110</t>
+  </si>
+  <si>
+    <t>000111</t>
+  </si>
+  <si>
+    <t>001000</t>
+  </si>
+  <si>
+    <t>001001</t>
   </si>
 </sst>
 </file>
@@ -1236,13 +1254,31 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1254,46 +1290,19 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1314,28 +1323,37 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2421,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K96" sqref="K96"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,11 +2480,11 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="99" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="120" t="s">
-        <v>62</v>
+      <c r="C3" s="100" t="s">
+        <v>162</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>103</v>
@@ -2485,8 +2503,8 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="114"/>
-      <c r="C4" s="104"/>
+      <c r="B4" s="88"/>
+      <c r="C4" s="94"/>
       <c r="D4" s="27" t="s">
         <v>106</v>
       </c>
@@ -2504,8 +2522,8 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="114"/>
-      <c r="C5" s="104"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="94"/>
       <c r="D5" s="25" t="s">
         <v>108</v>
       </c>
@@ -2523,8 +2541,8 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="115"/>
-      <c r="C6" s="96"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="95"/>
       <c r="D6" s="41" t="s">
         <v>110</v>
       </c>
@@ -2542,11 +2560,11 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="90" t="s">
-        <v>63</v>
+      <c r="C7" s="96" t="s">
+        <v>163</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>103</v>
@@ -2565,8 +2583,8 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="117"/>
-      <c r="C8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="97"/>
       <c r="D8" s="27" t="s">
         <v>106</v>
       </c>
@@ -2584,8 +2602,8 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="117"/>
-      <c r="C9" s="91"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="97"/>
       <c r="D9" s="25" t="s">
         <v>108</v>
       </c>
@@ -2603,8 +2621,8 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="118"/>
-      <c r="C10" s="92"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="98"/>
       <c r="D10" s="41" t="s">
         <v>110</v>
       </c>
@@ -2622,11 +2640,11 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="113" t="s">
+      <c r="B11" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="95" t="s">
-        <v>67</v>
+      <c r="C11" s="93" t="s">
+        <v>164</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>103</v>
@@ -2645,8 +2663,8 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="114"/>
-      <c r="C12" s="104"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="27" t="s">
         <v>106</v>
       </c>
@@ -2664,8 +2682,8 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="114"/>
-      <c r="C13" s="104"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="94"/>
       <c r="D13" s="25" t="s">
         <v>108</v>
       </c>
@@ -2683,8 +2701,8 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="115"/>
-      <c r="C14" s="96"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="95"/>
       <c r="D14" s="41" t="s">
         <v>110</v>
       </c>
@@ -2702,11 +2720,11 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="90" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="90" t="s">
-        <v>64</v>
+      <c r="C15" s="96" t="s">
+        <v>165</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>103</v>
@@ -2725,8 +2743,8 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="117"/>
-      <c r="C16" s="91"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="97"/>
       <c r="D16" s="27" t="s">
         <v>106</v>
       </c>
@@ -2744,8 +2762,8 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="117"/>
-      <c r="C17" s="91"/>
+      <c r="B17" s="91"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="25" t="s">
         <v>108</v>
       </c>
@@ -2763,8 +2781,8 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="118"/>
-      <c r="C18" s="92"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="98"/>
       <c r="D18" s="41" t="s">
         <v>110</v>
       </c>
@@ -2782,10 +2800,12 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="113" t="s">
+      <c r="B19" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="95"/>
+      <c r="C19" s="93" t="s">
+        <v>166</v>
+      </c>
       <c r="D19" s="30" t="s">
         <v>103</v>
       </c>
@@ -2803,8 +2823,8 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="114"/>
-      <c r="C20" s="104"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="94"/>
       <c r="D20" s="27" t="s">
         <v>106</v>
       </c>
@@ -2822,8 +2842,8 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="114"/>
-      <c r="C21" s="104"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="25" t="s">
         <v>108</v>
       </c>
@@ -2841,8 +2861,8 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="115"/>
-      <c r="C22" s="96"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="95"/>
       <c r="D22" s="41" t="s">
         <v>110</v>
       </c>
@@ -2860,10 +2880,12 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="116" t="s">
+      <c r="B23" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="C23" s="90"/>
+      <c r="C23" s="96" t="s">
+        <v>167</v>
+      </c>
       <c r="D23" s="30" t="s">
         <v>103</v>
       </c>
@@ -2881,8 +2903,8 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="117"/>
-      <c r="C24" s="91"/>
+      <c r="B24" s="91"/>
+      <c r="C24" s="97"/>
       <c r="D24" s="27" t="s">
         <v>106</v>
       </c>
@@ -2900,8 +2922,8 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="117"/>
-      <c r="C25" s="91"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="97"/>
       <c r="D25" s="25" t="s">
         <v>108</v>
       </c>
@@ -2919,8 +2941,8 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="118"/>
-      <c r="C26" s="92"/>
+      <c r="B26" s="92"/>
+      <c r="C26" s="98"/>
       <c r="D26" s="41" t="s">
         <v>110</v>
       </c>
@@ -2938,10 +2960,10 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="113" t="s">
+      <c r="B27" s="87" t="s">
         <v>124</v>
       </c>
-      <c r="C27" s="95" t="s">
+      <c r="C27" s="93" t="s">
         <v>68</v>
       </c>
       <c r="D27" s="30" t="s">
@@ -2961,8 +2983,8 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="114"/>
-      <c r="C28" s="104"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="94"/>
       <c r="D28" s="27" t="s">
         <v>106</v>
       </c>
@@ -2980,8 +3002,8 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="114"/>
-      <c r="C29" s="104"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="94"/>
       <c r="D29" s="25" t="s">
         <v>108</v>
       </c>
@@ -2999,8 +3021,8 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="115"/>
-      <c r="C30" s="96"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="95"/>
       <c r="D30" s="41" t="s">
         <v>110</v>
       </c>
@@ -3018,10 +3040,10 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="116" t="s">
+      <c r="B31" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="90" t="s">
+      <c r="C31" s="96" t="s">
         <v>69</v>
       </c>
       <c r="D31" s="30" t="s">
@@ -3041,8 +3063,8 @@
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="117"/>
-      <c r="C32" s="91"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="97"/>
       <c r="D32" s="27" t="s">
         <v>106</v>
       </c>
@@ -3060,8 +3082,8 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="117"/>
-      <c r="C33" s="91"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="97"/>
       <c r="D33" s="25" t="s">
         <v>108</v>
       </c>
@@ -3079,8 +3101,8 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="118"/>
-      <c r="C34" s="92"/>
+      <c r="B34" s="92"/>
+      <c r="C34" s="98"/>
       <c r="D34" s="41" t="s">
         <v>110</v>
       </c>
@@ -3098,10 +3120,10 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="93" t="s">
         <v>70</v>
       </c>
       <c r="D35" s="30" t="s">
@@ -3121,8 +3143,8 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="114"/>
-      <c r="C36" s="104"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="94"/>
       <c r="D36" s="27" t="s">
         <v>106</v>
       </c>
@@ -3140,8 +3162,8 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="114"/>
-      <c r="C37" s="104"/>
+      <c r="B37" s="88"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="25" t="s">
         <v>108</v>
       </c>
@@ -3159,8 +3181,8 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="115"/>
-      <c r="C38" s="96"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="95"/>
       <c r="D38" s="41" t="s">
         <v>110</v>
       </c>
@@ -3178,10 +3200,10 @@
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="90" t="s">
+      <c r="C39" s="96" t="s">
         <v>71</v>
       </c>
       <c r="D39" s="30" t="s">
@@ -3201,8 +3223,8 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="117"/>
-      <c r="C40" s="91"/>
+      <c r="B40" s="91"/>
+      <c r="C40" s="97"/>
       <c r="D40" s="27" t="s">
         <v>106</v>
       </c>
@@ -3220,8 +3242,8 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="117"/>
-      <c r="C41" s="91"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="97"/>
       <c r="D41" s="25" t="s">
         <v>108</v>
       </c>
@@ -3239,8 +3261,8 @@
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="118"/>
-      <c r="C42" s="92"/>
+      <c r="B42" s="92"/>
+      <c r="C42" s="98"/>
       <c r="D42" s="41" t="s">
         <v>110</v>
       </c>
@@ -3258,10 +3280,10 @@
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="113" t="s">
+      <c r="B43" s="87" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="95" t="s">
+      <c r="C43" s="93" t="s">
         <v>142</v>
       </c>
       <c r="D43" s="30" t="s">
@@ -3281,8 +3303,8 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="114"/>
-      <c r="C44" s="104"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="94"/>
       <c r="D44" s="27" t="s">
         <v>106</v>
       </c>
@@ -3300,8 +3322,8 @@
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="114"/>
-      <c r="C45" s="104"/>
+      <c r="B45" s="88"/>
+      <c r="C45" s="94"/>
       <c r="D45" s="25" t="s">
         <v>108</v>
       </c>
@@ -3319,8 +3341,8 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="115"/>
-      <c r="C46" s="96"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="95"/>
       <c r="D46" s="41" t="s">
         <v>110</v>
       </c>
@@ -3338,10 +3360,10 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="116" t="s">
+      <c r="B47" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="90" t="s">
+      <c r="C47" s="96" t="s">
         <v>72</v>
       </c>
       <c r="D47" s="30" t="s">
@@ -3361,8 +3383,8 @@
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="117"/>
-      <c r="C48" s="91"/>
+      <c r="B48" s="91"/>
+      <c r="C48" s="97"/>
       <c r="D48" s="27" t="s">
         <v>106</v>
       </c>
@@ -3380,8 +3402,8 @@
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="117"/>
-      <c r="C49" s="91"/>
+      <c r="B49" s="91"/>
+      <c r="C49" s="97"/>
       <c r="D49" s="25" t="s">
         <v>108</v>
       </c>
@@ -3399,8 +3421,8 @@
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="118"/>
-      <c r="C50" s="92"/>
+      <c r="B50" s="92"/>
+      <c r="C50" s="98"/>
       <c r="D50" s="41" t="s">
         <v>110</v>
       </c>
@@ -3418,10 +3440,10 @@
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="113" t="s">
+      <c r="B51" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="95" t="s">
+      <c r="C51" s="93" t="s">
         <v>73</v>
       </c>
       <c r="D51" s="30" t="s">
@@ -3441,8 +3463,8 @@
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="114"/>
-      <c r="C52" s="104"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="94"/>
       <c r="D52" s="27" t="s">
         <v>106</v>
       </c>
@@ -3460,8 +3482,8 @@
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="114"/>
-      <c r="C53" s="104"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="94"/>
       <c r="D53" s="25" t="s">
         <v>108</v>
       </c>
@@ -3479,8 +3501,8 @@
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="115"/>
-      <c r="C54" s="96"/>
+      <c r="B54" s="89"/>
+      <c r="C54" s="95"/>
       <c r="D54" s="41" t="s">
         <v>110</v>
       </c>
@@ -3498,10 +3520,10 @@
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="116" t="s">
+      <c r="B55" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="C55" s="90" t="s">
+      <c r="C55" s="96" t="s">
         <v>68</v>
       </c>
       <c r="D55" s="30" t="s">
@@ -3521,8 +3543,8 @@
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="117"/>
-      <c r="C56" s="91"/>
+      <c r="B56" s="91"/>
+      <c r="C56" s="97"/>
       <c r="D56" s="27" t="s">
         <v>106</v>
       </c>
@@ -3540,8 +3562,8 @@
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="117"/>
-      <c r="C57" s="91"/>
+      <c r="B57" s="91"/>
+      <c r="C57" s="97"/>
       <c r="D57" s="25" t="s">
         <v>108</v>
       </c>
@@ -3559,8 +3581,8 @@
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="118"/>
-      <c r="C58" s="92"/>
+      <c r="B58" s="92"/>
+      <c r="C58" s="98"/>
       <c r="D58" s="41" t="s">
         <v>110</v>
       </c>
@@ -3578,10 +3600,10 @@
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="113" t="s">
+      <c r="B59" s="87" t="s">
         <v>132</v>
       </c>
-      <c r="C59" s="95" t="s">
+      <c r="C59" s="93" t="s">
         <v>75</v>
       </c>
       <c r="D59" s="30" t="s">
@@ -3601,8 +3623,8 @@
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="114"/>
-      <c r="C60" s="104"/>
+      <c r="B60" s="88"/>
+      <c r="C60" s="94"/>
       <c r="D60" s="27" t="s">
         <v>106</v>
       </c>
@@ -3620,8 +3642,8 @@
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="114"/>
-      <c r="C61" s="104"/>
+      <c r="B61" s="88"/>
+      <c r="C61" s="94"/>
       <c r="D61" s="25" t="s">
         <v>108</v>
       </c>
@@ -3639,8 +3661,8 @@
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="115"/>
-      <c r="C62" s="96"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="95"/>
       <c r="D62" s="41" t="s">
         <v>110</v>
       </c>
@@ -3658,10 +3680,10 @@
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="116" t="s">
+      <c r="B63" s="90" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="90" t="s">
+      <c r="C63" s="96" t="s">
         <v>76</v>
       </c>
       <c r="D63" s="30" t="s">
@@ -3681,8 +3703,8 @@
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="117"/>
-      <c r="C64" s="91"/>
+      <c r="B64" s="91"/>
+      <c r="C64" s="97"/>
       <c r="D64" s="27" t="s">
         <v>106</v>
       </c>
@@ -3700,8 +3722,8 @@
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="117"/>
-      <c r="C65" s="91"/>
+      <c r="B65" s="91"/>
+      <c r="C65" s="97"/>
       <c r="D65" s="25" t="s">
         <v>108</v>
       </c>
@@ -3719,8 +3741,8 @@
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="118"/>
-      <c r="C66" s="92"/>
+      <c r="B66" s="92"/>
+      <c r="C66" s="98"/>
       <c r="D66" s="41" t="s">
         <v>110</v>
       </c>
@@ -3738,10 +3760,10 @@
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="113" t="s">
+      <c r="B67" s="87" t="s">
         <v>133</v>
       </c>
-      <c r="C67" s="95" t="s">
+      <c r="C67" s="93" t="s">
         <v>77</v>
       </c>
       <c r="D67" s="30" t="s">
@@ -3761,8 +3783,8 @@
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="114"/>
-      <c r="C68" s="104"/>
+      <c r="B68" s="88"/>
+      <c r="C68" s="94"/>
       <c r="D68" s="27" t="s">
         <v>106</v>
       </c>
@@ -3780,8 +3802,8 @@
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="114"/>
-      <c r="C69" s="104"/>
+      <c r="B69" s="88"/>
+      <c r="C69" s="94"/>
       <c r="D69" s="25" t="s">
         <v>108</v>
       </c>
@@ -3799,8 +3821,8 @@
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="115"/>
-      <c r="C70" s="96"/>
+      <c r="B70" s="89"/>
+      <c r="C70" s="95"/>
       <c r="D70" s="41" t="s">
         <v>110</v>
       </c>
@@ -3818,10 +3840,10 @@
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="87" t="s">
+      <c r="B71" s="101" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="90" t="s">
+      <c r="C71" s="96" t="s">
         <v>78</v>
       </c>
       <c r="D71" s="54" t="s">
@@ -3841,8 +3863,8 @@
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="88"/>
-      <c r="C72" s="91"/>
+      <c r="B72" s="102"/>
+      <c r="C72" s="97"/>
       <c r="D72" s="29" t="s">
         <v>106</v>
       </c>
@@ -3860,8 +3882,8 @@
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="88"/>
-      <c r="C73" s="91"/>
+      <c r="B73" s="102"/>
+      <c r="C73" s="97"/>
       <c r="D73" s="25" t="s">
         <v>108</v>
       </c>
@@ -3879,8 +3901,8 @@
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="89"/>
-      <c r="C74" s="92"/>
+      <c r="B74" s="103"/>
+      <c r="C74" s="98"/>
       <c r="D74" s="41" t="s">
         <v>110</v>
       </c>
@@ -3898,10 +3920,10 @@
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="107" t="s">
+      <c r="B75" s="104" t="s">
         <v>146</v>
       </c>
-      <c r="C75" s="110" t="s">
+      <c r="C75" s="107" t="s">
         <v>79</v>
       </c>
       <c r="D75" s="64" t="s">
@@ -3921,8 +3943,8 @@
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="108"/>
-      <c r="C76" s="111"/>
+      <c r="B76" s="105"/>
+      <c r="C76" s="108"/>
       <c r="D76" s="27" t="s">
         <v>147</v>
       </c>
@@ -3940,8 +3962,8 @@
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="109"/>
-      <c r="C77" s="112"/>
+      <c r="B77" s="106"/>
+      <c r="C77" s="109"/>
       <c r="D77" s="65" t="s">
         <v>110</v>
       </c>
@@ -3959,10 +3981,10 @@
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="87" t="s">
+      <c r="B78" s="101" t="s">
         <v>150</v>
       </c>
-      <c r="C78" s="90" t="s">
+      <c r="C78" s="96" t="s">
         <v>80</v>
       </c>
       <c r="D78" s="69" t="s">
@@ -3982,8 +4004,8 @@
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="88"/>
-      <c r="C79" s="91"/>
+      <c r="B79" s="102"/>
+      <c r="C79" s="97"/>
       <c r="D79" s="25" t="s">
         <v>106</v>
       </c>
@@ -4001,8 +4023,8 @@
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="88"/>
-      <c r="C80" s="91"/>
+      <c r="B80" s="102"/>
+      <c r="C80" s="97"/>
       <c r="D80" s="27" t="s">
         <v>108</v>
       </c>
@@ -4020,8 +4042,8 @@
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="88"/>
-      <c r="C81" s="91"/>
+      <c r="B81" s="102"/>
+      <c r="C81" s="97"/>
       <c r="D81" s="25" t="s">
         <v>147</v>
       </c>
@@ -4039,8 +4061,8 @@
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="89"/>
-      <c r="C82" s="92"/>
+      <c r="B82" s="103"/>
+      <c r="C82" s="98"/>
       <c r="D82" s="41" t="s">
         <v>110</v>
       </c>
@@ -4058,10 +4080,10 @@
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="103" t="s">
+      <c r="B83" s="110" t="s">
         <v>153</v>
       </c>
-      <c r="C83" s="104" t="s">
+      <c r="C83" s="94" t="s">
         <v>81</v>
       </c>
       <c r="D83" s="30" t="s">
@@ -4081,8 +4103,8 @@
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="103"/>
-      <c r="C84" s="104"/>
+      <c r="B84" s="110"/>
+      <c r="C84" s="94"/>
       <c r="D84" s="27" t="s">
         <v>106</v>
       </c>
@@ -4100,8 +4122,8 @@
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="103"/>
-      <c r="C85" s="104"/>
+      <c r="B85" s="110"/>
+      <c r="C85" s="94"/>
       <c r="D85" s="25" t="s">
         <v>108</v>
       </c>
@@ -4119,8 +4141,8 @@
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="103"/>
-      <c r="C86" s="104"/>
+      <c r="B86" s="110"/>
+      <c r="C86" s="94"/>
       <c r="D86" s="27" t="s">
         <v>147</v>
       </c>
@@ -4138,8 +4160,8 @@
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="94"/>
-      <c r="C87" s="96"/>
+      <c r="B87" s="111"/>
+      <c r="C87" s="95"/>
       <c r="D87" s="65" t="s">
         <v>152</v>
       </c>
@@ -4157,10 +4179,10 @@
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="97" t="s">
+      <c r="B88" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="C88" s="100" t="s">
+      <c r="C88" s="115" t="s">
         <v>82</v>
       </c>
       <c r="D88" s="60" t="s">
@@ -4180,8 +4202,8 @@
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="98"/>
-      <c r="C89" s="101"/>
+      <c r="B89" s="113"/>
+      <c r="C89" s="116"/>
       <c r="D89" s="25" t="s">
         <v>106</v>
       </c>
@@ -4199,8 +4221,8 @@
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="105"/>
-      <c r="C90" s="106"/>
+      <c r="B90" s="114"/>
+      <c r="C90" s="117"/>
       <c r="D90" s="41" t="s">
         <v>147</v>
       </c>
@@ -4218,10 +4240,10 @@
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="93" t="s">
+      <c r="B91" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="C91" s="95" t="s">
+      <c r="C91" s="93" t="s">
         <v>85</v>
       </c>
       <c r="D91" s="30" t="s">
@@ -4241,8 +4263,8 @@
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="103"/>
-      <c r="C92" s="104"/>
+      <c r="B92" s="110"/>
+      <c r="C92" s="94"/>
       <c r="D92" s="27" t="s">
         <v>106</v>
       </c>
@@ -4260,8 +4282,8 @@
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="103"/>
-      <c r="C93" s="104"/>
+      <c r="B93" s="110"/>
+      <c r="C93" s="94"/>
       <c r="D93" s="25" t="s">
         <v>108</v>
       </c>
@@ -4279,8 +4301,8 @@
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="94"/>
-      <c r="C94" s="96"/>
+      <c r="B94" s="111"/>
+      <c r="C94" s="95"/>
       <c r="D94" s="41" t="s">
         <v>147</v>
       </c>
@@ -4298,10 +4320,10 @@
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="87" t="s">
+      <c r="B95" s="101" t="s">
         <v>159</v>
       </c>
-      <c r="C95" s="90" t="s">
+      <c r="C95" s="96" t="s">
         <v>83</v>
       </c>
       <c r="D95" s="64" t="s">
@@ -4321,8 +4343,8 @@
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="88"/>
-      <c r="C96" s="91"/>
+      <c r="B96" s="102"/>
+      <c r="C96" s="97"/>
       <c r="D96" s="27" t="s">
         <v>106</v>
       </c>
@@ -4340,8 +4362,8 @@
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="88"/>
-      <c r="C97" s="91"/>
+      <c r="B97" s="102"/>
+      <c r="C97" s="97"/>
       <c r="D97" s="25" t="s">
         <v>108</v>
       </c>
@@ -4359,8 +4381,8 @@
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="89"/>
-      <c r="C98" s="92"/>
+      <c r="B98" s="103"/>
+      <c r="C98" s="98"/>
       <c r="D98" s="41" t="s">
         <v>147</v>
       </c>
@@ -4378,10 +4400,10 @@
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="93" t="s">
+      <c r="B99" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="C99" s="95" t="s">
+      <c r="C99" s="93" t="s">
         <v>84</v>
       </c>
       <c r="D99" s="64" t="s">
@@ -4401,8 +4423,8 @@
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="94"/>
-      <c r="C100" s="96"/>
+      <c r="B100" s="111"/>
+      <c r="C100" s="95"/>
       <c r="D100" s="41" t="s">
         <v>108</v>
       </c>
@@ -4420,10 +4442,10 @@
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="97" t="s">
+      <c r="B101" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="C101" s="100" t="s">
+      <c r="C101" s="115" t="s">
         <v>161</v>
       </c>
       <c r="D101" s="75" t="s">
@@ -4443,8 +4465,8 @@
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="98"/>
-      <c r="C102" s="101"/>
+      <c r="B102" s="113"/>
+      <c r="C102" s="116"/>
       <c r="D102" s="76" t="s">
         <v>106</v>
       </c>
@@ -4462,8 +4484,8 @@
       </c>
     </row>
     <row r="103" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="99"/>
-      <c r="C103" s="102"/>
+      <c r="B103" s="119"/>
+      <c r="C103" s="120"/>
       <c r="D103" s="83" t="s">
         <v>108</v>
       </c>
@@ -4689,6 +4711,46 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="C101:C103"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="C91:C94"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="C51:C54"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B46"/>
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C19:C22"/>
@@ -4701,46 +4763,6 @@
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="C51:C54"/>
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="B83:B87"/>
-    <mergeCell ref="C83:C87"/>
-    <mergeCell ref="B88:B90"/>
-    <mergeCell ref="C88:C90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="C91:C94"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="C101:C103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>